<commit_message>
updated CC_scattering_angle for CP05MOAS-GL335, 376 387
</commit_message>
<xml_diff>
--- a/deployment/Omaha_Cal_Info_CP05MOAS-GL335_00003.xlsx
+++ b/deployment/Omaha_Cal_Info_CP05MOAS-GL335_00003.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
-  <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="27127"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="660" yWindow="645" windowWidth="23205" windowHeight="8220" tabRatio="377" activeTab="1"/>
+    <workbookView xWindow="39920" yWindow="1620" windowWidth="30260" windowHeight="17340" tabRatio="377"/>
   </bookViews>
   <sheets>
     <sheet name="Moorings" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,12 @@
     <definedName name="_FilterDatabase_1_1_1">Moorings!$B$1:$K$99</definedName>
     <definedName name="_FilterDatabase_2">Asset_Cal_Info!$A$1:$H$386</definedName>
   </definedNames>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -860,22 +865,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K7" sqref="K7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="12.7109375" customWidth="1"/>
-    <col min="2" max="2" width="23.28515625" customWidth="1"/>
-    <col min="4" max="4" width="14.42578125" customWidth="1"/>
-    <col min="5" max="7" width="17.7109375" customWidth="1"/>
-    <col min="8" max="9" width="19.85546875" customWidth="1"/>
-    <col min="10" max="11" width="9.7109375" customWidth="1"/>
+    <col min="1" max="1" width="12.6640625" customWidth="1"/>
+    <col min="2" max="2" width="23.33203125" customWidth="1"/>
+    <col min="4" max="4" width="14.5" customWidth="1"/>
+    <col min="5" max="7" width="17.6640625" customWidth="1"/>
+    <col min="8" max="9" width="19.83203125" customWidth="1"/>
+    <col min="10" max="11" width="9.6640625" customWidth="1"/>
     <col min="12" max="12" width="18" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" ht="28">
       <c r="A1" s="24" t="s">
         <v>33</v>
       </c>
@@ -913,7 +918,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" s="4" customFormat="1" ht="15">
       <c r="A2" t="s">
         <v>34</v>
       </c>
@@ -959,17 +964,22 @@
         <v>-70.533333333333331</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14">
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14">
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="portrait"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -977,24 +987,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S19"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="80" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
+      <selection activeCell="H22" sqref="H22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="30.42578125" customWidth="1"/>
-    <col min="2" max="2" width="11.42578125" customWidth="1"/>
-    <col min="3" max="3" width="14.85546875" customWidth="1"/>
-    <col min="4" max="4" width="11.7109375" customWidth="1"/>
-    <col min="5" max="5" width="12.85546875" customWidth="1"/>
-    <col min="6" max="6" width="13.7109375" customWidth="1"/>
-    <col min="7" max="7" width="29.42578125" customWidth="1"/>
-    <col min="8" max="8" width="28.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="30.5" customWidth="1"/>
+    <col min="2" max="2" width="11.5" customWidth="1"/>
+    <col min="3" max="3" width="14.83203125" customWidth="1"/>
+    <col min="4" max="4" width="11.6640625" customWidth="1"/>
+    <col min="5" max="5" width="12.83203125" customWidth="1"/>
+    <col min="6" max="6" width="13.6640625" customWidth="1"/>
+    <col min="7" max="7" width="29.5" customWidth="1"/>
+    <col min="8" max="8" width="28.83203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" ht="28">
       <c r="A1" s="25" t="s">
         <v>0</v>
       </c>
@@ -1020,7 +1030,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:19">
       <c r="A2" s="7" t="s">
         <v>27</v>
       </c>
@@ -1059,7 +1069,7 @@
       <c r="R2" s="13"/>
       <c r="S2" s="13"/>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:19">
       <c r="A3" s="3" t="s">
         <v>27</v>
       </c>
@@ -1098,7 +1108,7 @@
       <c r="R3" s="13"/>
       <c r="S3" s="13"/>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:19">
       <c r="A4" s="3" t="s">
         <v>27</v>
       </c>
@@ -1137,7 +1147,7 @@
       <c r="R4" s="13"/>
       <c r="S4" s="13"/>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:19">
       <c r="A5" s="3" t="s">
         <v>27</v>
       </c>
@@ -1176,7 +1186,7 @@
       <c r="R5" s="13"/>
       <c r="S5" s="13"/>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:19">
       <c r="A6" s="3"/>
       <c r="B6" s="3"/>
       <c r="C6" s="10"/>
@@ -1197,7 +1207,7 @@
       <c r="R6" s="13"/>
       <c r="S6" s="13"/>
     </row>
-    <row r="7" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:19" s="2" customFormat="1">
       <c r="A7" s="7" t="s">
         <v>28</v>
       </c>
@@ -1220,7 +1230,7 @@
         <v>20</v>
       </c>
       <c r="H7" s="17">
-        <v>117</v>
+        <v>124</v>
       </c>
       <c r="I7" s="8" t="s">
         <v>19</v>
@@ -1231,7 +1241,7 @@
       <c r="M7" s="8"/>
       <c r="N7" s="8"/>
     </row>
-    <row r="8" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:19" s="2" customFormat="1">
       <c r="A8" s="3" t="s">
         <v>28</v>
       </c>
@@ -1265,7 +1275,7 @@
       <c r="M8" s="8"/>
       <c r="N8" s="8"/>
     </row>
-    <row r="9" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:19" s="2" customFormat="1">
       <c r="A9" s="3" t="s">
         <v>28</v>
       </c>
@@ -1299,7 +1309,7 @@
       <c r="M9" s="8"/>
       <c r="N9" s="8"/>
     </row>
-    <row r="10" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:19" s="2" customFormat="1">
       <c r="A10" s="3" t="s">
         <v>28</v>
       </c>
@@ -1333,7 +1343,7 @@
       <c r="M10" s="8"/>
       <c r="N10" s="8"/>
     </row>
-    <row r="11" spans="1:19" s="2" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:19" s="2" customFormat="1">
       <c r="A11" s="3"/>
       <c r="B11" s="3"/>
       <c r="C11" s="10"/>
@@ -1349,7 +1359,7 @@
       <c r="M11" s="8"/>
       <c r="N11" s="8"/>
     </row>
-    <row r="12" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:19" s="2" customFormat="1">
       <c r="A12" s="7" t="s">
         <v>29</v>
       </c>
@@ -1379,7 +1389,7 @@
       <c r="M12" s="8"/>
       <c r="N12" s="8"/>
     </row>
-    <row r="13" spans="1:19" s="2" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:19" s="2" customFormat="1">
       <c r="A13" s="7"/>
       <c r="B13" s="7"/>
       <c r="C13" s="10"/>
@@ -1395,7 +1405,7 @@
       <c r="M13" s="8"/>
       <c r="N13" s="8"/>
     </row>
-    <row r="14" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:19" s="2" customFormat="1">
       <c r="A14" s="7" t="s">
         <v>30</v>
       </c>
@@ -1425,7 +1435,7 @@
       <c r="M14" s="8"/>
       <c r="N14" s="8"/>
     </row>
-    <row r="15" spans="1:19" s="2" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:19" s="2" customFormat="1">
       <c r="A15" s="7"/>
       <c r="B15" s="7"/>
       <c r="C15" s="10"/>
@@ -1441,7 +1451,7 @@
       <c r="M15" s="8"/>
       <c r="N15" s="8"/>
     </row>
-    <row r="16" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:19" s="2" customFormat="1">
       <c r="A16" s="7" t="s">
         <v>31</v>
       </c>
@@ -1475,7 +1485,7 @@
       <c r="M16" s="8"/>
       <c r="N16" s="8"/>
     </row>
-    <row r="17" spans="1:14" s="2" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:14" s="2" customFormat="1">
       <c r="A17" s="7"/>
       <c r="B17" s="7"/>
       <c r="C17" s="10"/>
@@ -1491,7 +1501,7 @@
       <c r="M17" s="8"/>
       <c r="N17" s="8"/>
     </row>
-    <row r="18" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:14" s="2" customFormat="1">
       <c r="A18" s="7" t="s">
         <v>32</v>
       </c>
@@ -1521,7 +1531,7 @@
       <c r="M18" s="8"/>
       <c r="N18" s="8"/>
     </row>
-    <row r="19" spans="1:14" s="2" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:14" s="2" customFormat="1">
       <c r="A19" s="8"/>
       <c r="B19" s="8"/>
       <c r="C19" s="10"/>

</xml_diff>